<commit_message>
Revisi Program dan Dokumen
</commit_message>
<xml_diff>
--- a/hasil/xls/sampel108052017.xlsx
+++ b/hasil/xls/sampel108052017.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="sampel108052017" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
@@ -602,7 +599,7 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1936,7 +1933,7 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -8691,2372 +8688,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="sampel115052017"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="C1">
-            <v>33</v>
-          </cell>
-          <cell r="D1">
-            <v>28</v>
-          </cell>
-          <cell r="E1">
-            <v>42</v>
-          </cell>
-          <cell r="F1">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="C2">
-            <v>32</v>
-          </cell>
-          <cell r="D2">
-            <v>29</v>
-          </cell>
-          <cell r="E2">
-            <v>40</v>
-          </cell>
-          <cell r="F2">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="C3">
-            <v>32</v>
-          </cell>
-          <cell r="D3">
-            <v>29</v>
-          </cell>
-          <cell r="E3">
-            <v>37</v>
-          </cell>
-          <cell r="F3">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="C4">
-            <v>31</v>
-          </cell>
-          <cell r="D4">
-            <v>28</v>
-          </cell>
-          <cell r="E4">
-            <v>36</v>
-          </cell>
-          <cell r="F4">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5">
-            <v>31</v>
-          </cell>
-          <cell r="D5">
-            <v>27</v>
-          </cell>
-          <cell r="E5">
-            <v>36</v>
-          </cell>
-          <cell r="F5">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>32</v>
-          </cell>
-          <cell r="D6">
-            <v>28</v>
-          </cell>
-          <cell r="E6">
-            <v>38</v>
-          </cell>
-          <cell r="F6">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>36</v>
-          </cell>
-          <cell r="D7">
-            <v>30</v>
-          </cell>
-          <cell r="E7">
-            <v>47</v>
-          </cell>
-          <cell r="F7">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>39</v>
-          </cell>
-          <cell r="D8">
-            <v>31</v>
-          </cell>
-          <cell r="E8">
-            <v>55</v>
-          </cell>
-          <cell r="F8">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9">
-            <v>39</v>
-          </cell>
-          <cell r="D9">
-            <v>32</v>
-          </cell>
-          <cell r="E9">
-            <v>54</v>
-          </cell>
-          <cell r="F9">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>40</v>
-          </cell>
-          <cell r="D10">
-            <v>33</v>
-          </cell>
-          <cell r="E10">
-            <v>57</v>
-          </cell>
-          <cell r="F10">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>43</v>
-          </cell>
-          <cell r="D11">
-            <v>35</v>
-          </cell>
-          <cell r="E11">
-            <v>63</v>
-          </cell>
-          <cell r="F11">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>44</v>
-          </cell>
-          <cell r="D12">
-            <v>36</v>
-          </cell>
-          <cell r="E12">
-            <v>66</v>
-          </cell>
-          <cell r="F12">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>44</v>
-          </cell>
-          <cell r="D13">
-            <v>35</v>
-          </cell>
-          <cell r="E13">
-            <v>64</v>
-          </cell>
-          <cell r="F13">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>45</v>
-          </cell>
-          <cell r="D14">
-            <v>36</v>
-          </cell>
-          <cell r="E14">
-            <v>69</v>
-          </cell>
-          <cell r="F14">
-            <v>14</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>48</v>
-          </cell>
-          <cell r="D15">
-            <v>37</v>
-          </cell>
-          <cell r="E15">
-            <v>72</v>
-          </cell>
-          <cell r="F15">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>49</v>
-          </cell>
-          <cell r="D16">
-            <v>38</v>
-          </cell>
-          <cell r="E16">
-            <v>73</v>
-          </cell>
-          <cell r="F16">
-            <v>16</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>49</v>
-          </cell>
-          <cell r="D17">
-            <v>39</v>
-          </cell>
-          <cell r="E17">
-            <v>77</v>
-          </cell>
-          <cell r="F17">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>53</v>
-          </cell>
-          <cell r="D18">
-            <v>42</v>
-          </cell>
-          <cell r="E18">
-            <v>78</v>
-          </cell>
-          <cell r="F18">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>46</v>
-          </cell>
-          <cell r="D19">
-            <v>37</v>
-          </cell>
-          <cell r="E19">
-            <v>67</v>
-          </cell>
-          <cell r="F19">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>43</v>
-          </cell>
-          <cell r="D20">
-            <v>35</v>
-          </cell>
-          <cell r="E20">
-            <v>61</v>
-          </cell>
-          <cell r="F20">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>41</v>
-          </cell>
-          <cell r="D21">
-            <v>34</v>
-          </cell>
-          <cell r="E21">
-            <v>57</v>
-          </cell>
-          <cell r="F21">
-            <v>21</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>40</v>
-          </cell>
-          <cell r="D22">
-            <v>33</v>
-          </cell>
-          <cell r="E22">
-            <v>54</v>
-          </cell>
-          <cell r="F22">
-            <v>22</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>38</v>
-          </cell>
-          <cell r="D23">
-            <v>31</v>
-          </cell>
-          <cell r="E23">
-            <v>49</v>
-          </cell>
-          <cell r="F23">
-            <v>23</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>35</v>
-          </cell>
-          <cell r="D24">
-            <v>30</v>
-          </cell>
-          <cell r="E24">
-            <v>45</v>
-          </cell>
-          <cell r="F24">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>34</v>
-          </cell>
-          <cell r="D25">
-            <v>29</v>
-          </cell>
-          <cell r="E25">
-            <v>42</v>
-          </cell>
-          <cell r="F25">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>32</v>
-          </cell>
-          <cell r="D26">
-            <v>28</v>
-          </cell>
-          <cell r="E26">
-            <v>40</v>
-          </cell>
-          <cell r="F26">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>31</v>
-          </cell>
-          <cell r="D27">
-            <v>29</v>
-          </cell>
-          <cell r="E27">
-            <v>37</v>
-          </cell>
-          <cell r="F27">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>31</v>
-          </cell>
-          <cell r="D28">
-            <v>28</v>
-          </cell>
-          <cell r="E28">
-            <v>36</v>
-          </cell>
-          <cell r="F28">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29">
-            <v>31</v>
-          </cell>
-          <cell r="D29">
-            <v>28</v>
-          </cell>
-          <cell r="E29">
-            <v>35</v>
-          </cell>
-          <cell r="F29">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30">
-            <v>32</v>
-          </cell>
-          <cell r="D30">
-            <v>28</v>
-          </cell>
-          <cell r="E30">
-            <v>37</v>
-          </cell>
-          <cell r="F30">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31">
-            <v>36</v>
-          </cell>
-          <cell r="D31">
-            <v>30</v>
-          </cell>
-          <cell r="E31">
-            <v>47</v>
-          </cell>
-          <cell r="F31">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32">
-            <v>39</v>
-          </cell>
-          <cell r="D32">
-            <v>32</v>
-          </cell>
-          <cell r="E32">
-            <v>55</v>
-          </cell>
-          <cell r="F32">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>39</v>
-          </cell>
-          <cell r="D33">
-            <v>32</v>
-          </cell>
-          <cell r="E33">
-            <v>55</v>
-          </cell>
-          <cell r="F33">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>40</v>
-          </cell>
-          <cell r="D34">
-            <v>33</v>
-          </cell>
-          <cell r="E34">
-            <v>56</v>
-          </cell>
-          <cell r="F34">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>43</v>
-          </cell>
-          <cell r="D35">
-            <v>34</v>
-          </cell>
-          <cell r="E35">
-            <v>62</v>
-          </cell>
-          <cell r="F35">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36">
-            <v>44</v>
-          </cell>
-          <cell r="D36">
-            <v>35</v>
-          </cell>
-          <cell r="E36">
-            <v>63</v>
-          </cell>
-          <cell r="F36">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>45</v>
-          </cell>
-          <cell r="D37">
-            <v>36</v>
-          </cell>
-          <cell r="E37">
-            <v>65</v>
-          </cell>
-          <cell r="F37">
-            <v>14</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>46</v>
-          </cell>
-          <cell r="D38">
-            <v>37</v>
-          </cell>
-          <cell r="E38">
-            <v>71</v>
-          </cell>
-          <cell r="F38">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39">
-            <v>48</v>
-          </cell>
-          <cell r="D39">
-            <v>38</v>
-          </cell>
-          <cell r="E39">
-            <v>71</v>
-          </cell>
-          <cell r="F39">
-            <v>16</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40">
-            <v>48</v>
-          </cell>
-          <cell r="D40">
-            <v>38</v>
-          </cell>
-          <cell r="E40">
-            <v>71</v>
-          </cell>
-          <cell r="F40">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41">
-            <v>50</v>
-          </cell>
-          <cell r="D41">
-            <v>39</v>
-          </cell>
-          <cell r="E41">
-            <v>76</v>
-          </cell>
-          <cell r="F41">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42">
-            <v>54</v>
-          </cell>
-          <cell r="D42">
-            <v>42</v>
-          </cell>
-          <cell r="E42">
-            <v>79</v>
-          </cell>
-          <cell r="F42">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="C43">
-            <v>46</v>
-          </cell>
-          <cell r="D43">
-            <v>38</v>
-          </cell>
-          <cell r="E43">
-            <v>67</v>
-          </cell>
-          <cell r="F43">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="C44">
-            <v>44</v>
-          </cell>
-          <cell r="D44">
-            <v>36</v>
-          </cell>
-          <cell r="E44">
-            <v>63</v>
-          </cell>
-          <cell r="F44">
-            <v>21</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="C45">
-            <v>42</v>
-          </cell>
-          <cell r="D45">
-            <v>35</v>
-          </cell>
-          <cell r="E45">
-            <v>59</v>
-          </cell>
-          <cell r="F45">
-            <v>22</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="C46">
-            <v>41</v>
-          </cell>
-          <cell r="D46">
-            <v>34</v>
-          </cell>
-          <cell r="E46">
-            <v>55</v>
-          </cell>
-          <cell r="F46">
-            <v>23</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="C47">
-            <v>38</v>
-          </cell>
-          <cell r="D47">
-            <v>32</v>
-          </cell>
-          <cell r="E47">
-            <v>50</v>
-          </cell>
-          <cell r="F47">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="C48">
-            <v>35</v>
-          </cell>
-          <cell r="D48">
-            <v>30</v>
-          </cell>
-          <cell r="E48">
-            <v>45</v>
-          </cell>
-          <cell r="F48">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="C49">
-            <v>34</v>
-          </cell>
-          <cell r="D49">
-            <v>29</v>
-          </cell>
-          <cell r="E49">
-            <v>42</v>
-          </cell>
-          <cell r="F49">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="C50">
-            <v>33</v>
-          </cell>
-          <cell r="D50">
-            <v>29</v>
-          </cell>
-          <cell r="E50">
-            <v>40</v>
-          </cell>
-          <cell r="F50">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="C51">
-            <v>32</v>
-          </cell>
-          <cell r="D51">
-            <v>29</v>
-          </cell>
-          <cell r="E51">
-            <v>37</v>
-          </cell>
-          <cell r="F51">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="C52">
-            <v>31</v>
-          </cell>
-          <cell r="D52">
-            <v>28</v>
-          </cell>
-          <cell r="E52">
-            <v>36</v>
-          </cell>
-          <cell r="F52">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="C53">
-            <v>30</v>
-          </cell>
-          <cell r="D53">
-            <v>28</v>
-          </cell>
-          <cell r="E53">
-            <v>34</v>
-          </cell>
-          <cell r="F53">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="C54">
-            <v>33</v>
-          </cell>
-          <cell r="D54">
-            <v>29</v>
-          </cell>
-          <cell r="E54">
-            <v>38</v>
-          </cell>
-          <cell r="F54">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="C55">
-            <v>36</v>
-          </cell>
-          <cell r="D55">
-            <v>30</v>
-          </cell>
-          <cell r="E55">
-            <v>49</v>
-          </cell>
-          <cell r="F55">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="C56">
-            <v>39</v>
-          </cell>
-          <cell r="D56">
-            <v>32</v>
-          </cell>
-          <cell r="E56">
-            <v>56</v>
-          </cell>
-          <cell r="F56">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="C57">
-            <v>40</v>
-          </cell>
-          <cell r="D57">
-            <v>32</v>
-          </cell>
-          <cell r="E57">
-            <v>56</v>
-          </cell>
-          <cell r="F57">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="C58">
-            <v>41</v>
-          </cell>
-          <cell r="D58">
-            <v>33</v>
-          </cell>
-          <cell r="E58">
-            <v>58</v>
-          </cell>
-          <cell r="F58">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="C59">
-            <v>44</v>
-          </cell>
-          <cell r="D59">
-            <v>35</v>
-          </cell>
-          <cell r="E59">
-            <v>63</v>
-          </cell>
-          <cell r="F59">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="C60">
-            <v>44</v>
-          </cell>
-          <cell r="D60">
-            <v>35</v>
-          </cell>
-          <cell r="E60">
-            <v>65</v>
-          </cell>
-          <cell r="F60">
-            <v>14</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="C61">
-            <v>44</v>
-          </cell>
-          <cell r="D61">
-            <v>36</v>
-          </cell>
-          <cell r="E61">
-            <v>64</v>
-          </cell>
-          <cell r="F61">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="C62">
-            <v>47</v>
-          </cell>
-          <cell r="D62">
-            <v>37</v>
-          </cell>
-          <cell r="E62">
-            <v>70</v>
-          </cell>
-          <cell r="F62">
-            <v>16</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="C63">
-            <v>48</v>
-          </cell>
-          <cell r="D63">
-            <v>38</v>
-          </cell>
-          <cell r="E63">
-            <v>73</v>
-          </cell>
-          <cell r="F63">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="C64">
-            <v>50</v>
-          </cell>
-          <cell r="D64">
-            <v>39</v>
-          </cell>
-          <cell r="E64">
-            <v>73</v>
-          </cell>
-          <cell r="F64">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="C65">
-            <v>50</v>
-          </cell>
-          <cell r="D65">
-            <v>40</v>
-          </cell>
-          <cell r="E65">
-            <v>79</v>
-          </cell>
-          <cell r="F65">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="C66">
-            <v>54</v>
-          </cell>
-          <cell r="D66">
-            <v>43</v>
-          </cell>
-          <cell r="E66">
-            <v>82</v>
-          </cell>
-          <cell r="F66">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="C67">
-            <v>48</v>
-          </cell>
-          <cell r="D67">
-            <v>39</v>
-          </cell>
-          <cell r="E67">
-            <v>69</v>
-          </cell>
-          <cell r="F67">
-            <v>21</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="C68">
-            <v>44</v>
-          </cell>
-          <cell r="D68">
-            <v>36</v>
-          </cell>
-          <cell r="E68">
-            <v>63</v>
-          </cell>
-          <cell r="F68">
-            <v>22</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="C69">
-            <v>43</v>
-          </cell>
-          <cell r="D69">
-            <v>35</v>
-          </cell>
-          <cell r="E69">
-            <v>59</v>
-          </cell>
-          <cell r="F69">
-            <v>23</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="C70">
-            <v>41</v>
-          </cell>
-          <cell r="D70">
-            <v>34</v>
-          </cell>
-          <cell r="E70">
-            <v>59</v>
-          </cell>
-          <cell r="F70">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="C71">
-            <v>38</v>
-          </cell>
-          <cell r="D71">
-            <v>32</v>
-          </cell>
-          <cell r="E71">
-            <v>51</v>
-          </cell>
-          <cell r="F71">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="C72">
-            <v>35</v>
-          </cell>
-          <cell r="D72">
-            <v>30</v>
-          </cell>
-          <cell r="E72">
-            <v>46</v>
-          </cell>
-          <cell r="F72">
-            <v>26</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="C73">
-            <v>34</v>
-          </cell>
-          <cell r="D73">
-            <v>29</v>
-          </cell>
-          <cell r="E73">
-            <v>42</v>
-          </cell>
-          <cell r="F73">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="C74">
-            <v>33</v>
-          </cell>
-          <cell r="D74">
-            <v>29</v>
-          </cell>
-          <cell r="E74">
-            <v>41</v>
-          </cell>
-          <cell r="F74">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="C75">
-            <v>32</v>
-          </cell>
-          <cell r="D75">
-            <v>28</v>
-          </cell>
-          <cell r="E75">
-            <v>37</v>
-          </cell>
-          <cell r="F75">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="C76">
-            <v>32</v>
-          </cell>
-          <cell r="D76">
-            <v>29</v>
-          </cell>
-          <cell r="E76">
-            <v>37</v>
-          </cell>
-          <cell r="F76">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="C77">
-            <v>31</v>
-          </cell>
-          <cell r="D77">
-            <v>28</v>
-          </cell>
-          <cell r="E77">
-            <v>36</v>
-          </cell>
-          <cell r="F77">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="C78">
-            <v>33</v>
-          </cell>
-          <cell r="D78">
-            <v>29</v>
-          </cell>
-          <cell r="E78">
-            <v>38</v>
-          </cell>
-          <cell r="F78">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="C79">
-            <v>37</v>
-          </cell>
-          <cell r="D79">
-            <v>30</v>
-          </cell>
-          <cell r="E79">
-            <v>48</v>
-          </cell>
-          <cell r="F79">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="C80">
-            <v>39</v>
-          </cell>
-          <cell r="D80">
-            <v>32</v>
-          </cell>
-          <cell r="E80">
-            <v>56</v>
-          </cell>
-          <cell r="F80">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="C81">
-            <v>40</v>
-          </cell>
-          <cell r="D81">
-            <v>33</v>
-          </cell>
-          <cell r="E81">
-            <v>55</v>
-          </cell>
-          <cell r="F81">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="C82">
-            <v>41</v>
-          </cell>
-          <cell r="D82">
-            <v>33</v>
-          </cell>
-          <cell r="E82">
-            <v>58</v>
-          </cell>
-          <cell r="F82">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="C83">
-            <v>44</v>
-          </cell>
-          <cell r="D83">
-            <v>35</v>
-          </cell>
-          <cell r="E83">
-            <v>63</v>
-          </cell>
-          <cell r="F83">
-            <v>14</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="C84">
-            <v>45</v>
-          </cell>
-          <cell r="D84">
-            <v>36</v>
-          </cell>
-          <cell r="E84">
-            <v>66</v>
-          </cell>
-          <cell r="F84">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="C85">
-            <v>45</v>
-          </cell>
-          <cell r="D85">
-            <v>36</v>
-          </cell>
-          <cell r="E85">
-            <v>66</v>
-          </cell>
-          <cell r="F85">
-            <v>16</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="C86">
-            <v>47</v>
-          </cell>
-          <cell r="D86">
-            <v>37</v>
-          </cell>
-          <cell r="E86">
-            <v>71</v>
-          </cell>
-          <cell r="F86">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="C87">
-            <v>49</v>
-          </cell>
-          <cell r="D87">
-            <v>39</v>
-          </cell>
-          <cell r="E87">
-            <v>74</v>
-          </cell>
-          <cell r="F87">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="C88">
-            <v>49</v>
-          </cell>
-          <cell r="D88">
-            <v>39</v>
-          </cell>
-          <cell r="E88">
-            <v>72</v>
-          </cell>
-          <cell r="F88">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="C89">
-            <v>50</v>
-          </cell>
-          <cell r="D89">
-            <v>40</v>
-          </cell>
-          <cell r="E89">
-            <v>77</v>
-          </cell>
-          <cell r="F89">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="C90">
-            <v>53</v>
-          </cell>
-          <cell r="D90">
-            <v>42</v>
-          </cell>
-          <cell r="E90">
-            <v>78</v>
-          </cell>
-          <cell r="F90">
-            <v>21</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="C91">
-            <v>46</v>
-          </cell>
-          <cell r="D91">
-            <v>37</v>
-          </cell>
-          <cell r="E91">
-            <v>68</v>
-          </cell>
-          <cell r="F91">
-            <v>22</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="C92">
-            <v>45</v>
-          </cell>
-          <cell r="D92">
-            <v>37</v>
-          </cell>
-          <cell r="E92">
-            <v>64</v>
-          </cell>
-          <cell r="F92">
-            <v>23</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="C93">
-            <v>43</v>
-          </cell>
-          <cell r="D93">
-            <v>35</v>
-          </cell>
-          <cell r="E93">
-            <v>61</v>
-          </cell>
-          <cell r="F93">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="C94">
-            <v>42</v>
-          </cell>
-          <cell r="D94">
-            <v>34</v>
-          </cell>
-          <cell r="E94">
-            <v>57</v>
-          </cell>
-          <cell r="F94">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="C95">
-            <v>38</v>
-          </cell>
-          <cell r="D95">
-            <v>32</v>
-          </cell>
-          <cell r="E95">
-            <v>51</v>
-          </cell>
-          <cell r="F95">
-            <v>26</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="C96">
-            <v>35</v>
-          </cell>
-          <cell r="D96">
-            <v>30</v>
-          </cell>
-          <cell r="E96">
-            <v>46</v>
-          </cell>
-          <cell r="F96">
-            <v>27</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="C97">
-            <v>33</v>
-          </cell>
-          <cell r="D97">
-            <v>29</v>
-          </cell>
-          <cell r="E97">
-            <v>42</v>
-          </cell>
-          <cell r="F97">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="C98">
-            <v>33</v>
-          </cell>
-          <cell r="D98">
-            <v>28</v>
-          </cell>
-          <cell r="E98">
-            <v>42</v>
-          </cell>
-          <cell r="F98">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="C99">
-            <v>32</v>
-          </cell>
-          <cell r="D99">
-            <v>29</v>
-          </cell>
-          <cell r="E99">
-            <v>39</v>
-          </cell>
-          <cell r="F99">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="C100">
-            <v>32</v>
-          </cell>
-          <cell r="D100">
-            <v>28</v>
-          </cell>
-          <cell r="E100">
-            <v>37</v>
-          </cell>
-          <cell r="F100">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="C101">
-            <v>31</v>
-          </cell>
-          <cell r="D101">
-            <v>28</v>
-          </cell>
-          <cell r="E101">
-            <v>36</v>
-          </cell>
-          <cell r="F101">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="C102">
-            <v>33</v>
-          </cell>
-          <cell r="D102">
-            <v>29</v>
-          </cell>
-          <cell r="E102">
-            <v>39</v>
-          </cell>
-          <cell r="F102">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="C103">
-            <v>36</v>
-          </cell>
-          <cell r="D103">
-            <v>30</v>
-          </cell>
-          <cell r="E103">
-            <v>48</v>
-          </cell>
-          <cell r="F103">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="C104">
-            <v>39</v>
-          </cell>
-          <cell r="D104">
-            <v>32</v>
-          </cell>
-          <cell r="E104">
-            <v>56</v>
-          </cell>
-          <cell r="F104">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="C105">
-            <v>40</v>
-          </cell>
-          <cell r="D105">
-            <v>33</v>
-          </cell>
-          <cell r="E105">
-            <v>57</v>
-          </cell>
-          <cell r="F105">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="C106">
-            <v>41</v>
-          </cell>
-          <cell r="D106">
-            <v>33</v>
-          </cell>
-          <cell r="E106">
-            <v>59</v>
-          </cell>
-          <cell r="F106">
-            <v>14</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="C107">
-            <v>44</v>
-          </cell>
-          <cell r="D107">
-            <v>35</v>
-          </cell>
-          <cell r="E107">
-            <v>64</v>
-          </cell>
-          <cell r="F107">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="C108">
-            <v>46</v>
-          </cell>
-          <cell r="D108">
-            <v>37</v>
-          </cell>
-          <cell r="E108">
-            <v>68</v>
-          </cell>
-          <cell r="F108">
-            <v>16</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="C109">
-            <v>41</v>
-          </cell>
-          <cell r="D109">
-            <v>33</v>
-          </cell>
-          <cell r="E109">
-            <v>57</v>
-          </cell>
-          <cell r="F109">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="C110">
-            <v>46</v>
-          </cell>
-          <cell r="D110">
-            <v>36</v>
-          </cell>
-          <cell r="E110">
-            <v>71</v>
-          </cell>
-          <cell r="F110">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="C111">
-            <v>50</v>
-          </cell>
-          <cell r="D111">
-            <v>39</v>
-          </cell>
-          <cell r="E111">
-            <v>75</v>
-          </cell>
-          <cell r="F111">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="C112">
-            <v>49</v>
-          </cell>
-          <cell r="D112">
-            <v>39</v>
-          </cell>
-          <cell r="E112">
-            <v>74</v>
-          </cell>
-          <cell r="F112">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="C113">
-            <v>52</v>
-          </cell>
-          <cell r="D113">
-            <v>40</v>
-          </cell>
-          <cell r="E113">
-            <v>82</v>
-          </cell>
-          <cell r="F113">
-            <v>21</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="C114">
-            <v>57</v>
-          </cell>
-          <cell r="D114">
-            <v>44</v>
-          </cell>
-          <cell r="E114">
-            <v>85</v>
-          </cell>
-          <cell r="F114">
-            <v>22</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="C115">
-            <v>51</v>
-          </cell>
-          <cell r="D115">
-            <v>40</v>
-          </cell>
-          <cell r="E115">
-            <v>74</v>
-          </cell>
-          <cell r="F115">
-            <v>23</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="C116">
-            <v>48</v>
-          </cell>
-          <cell r="D116">
-            <v>38</v>
-          </cell>
-          <cell r="E116">
-            <v>69</v>
-          </cell>
-          <cell r="F116">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="C117">
-            <v>45</v>
-          </cell>
-          <cell r="D117">
-            <v>36</v>
-          </cell>
-          <cell r="E117">
-            <v>66</v>
-          </cell>
-          <cell r="F117">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="C118">
-            <v>44</v>
-          </cell>
-          <cell r="D118">
-            <v>36</v>
-          </cell>
-          <cell r="E118">
-            <v>61</v>
-          </cell>
-          <cell r="F118">
-            <v>26</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="C119">
-            <v>41</v>
-          </cell>
-          <cell r="D119">
-            <v>34</v>
-          </cell>
-          <cell r="E119">
-            <v>57</v>
-          </cell>
-          <cell r="F119">
-            <v>27</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="C120">
-            <v>37</v>
-          </cell>
-          <cell r="D120">
-            <v>31</v>
-          </cell>
-          <cell r="E120">
-            <v>49</v>
-          </cell>
-          <cell r="F120">
-            <v>28</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="C121">
-            <v>34</v>
-          </cell>
-          <cell r="D121">
-            <v>30</v>
-          </cell>
-          <cell r="E121">
-            <v>44</v>
-          </cell>
-          <cell r="F121">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="C122">
-            <v>34</v>
-          </cell>
-          <cell r="D122">
-            <v>29</v>
-          </cell>
-          <cell r="E122">
-            <v>42</v>
-          </cell>
-          <cell r="F122">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="C123">
-            <v>32</v>
-          </cell>
-          <cell r="D123">
-            <v>28</v>
-          </cell>
-          <cell r="E123">
-            <v>40</v>
-          </cell>
-          <cell r="F123">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="C124">
-            <v>32</v>
-          </cell>
-          <cell r="D124">
-            <v>28</v>
-          </cell>
-          <cell r="E124">
-            <v>38</v>
-          </cell>
-          <cell r="F124">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="C125">
-            <v>32</v>
-          </cell>
-          <cell r="D125">
-            <v>28</v>
-          </cell>
-          <cell r="E125">
-            <v>40</v>
-          </cell>
-          <cell r="F125">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="C126">
-            <v>33</v>
-          </cell>
-          <cell r="D126">
-            <v>28</v>
-          </cell>
-          <cell r="E126">
-            <v>41</v>
-          </cell>
-          <cell r="F126">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="C127">
-            <v>34</v>
-          </cell>
-          <cell r="D127">
-            <v>29</v>
-          </cell>
-          <cell r="E127">
-            <v>45</v>
-          </cell>
-          <cell r="F127">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="C128">
-            <v>36</v>
-          </cell>
-          <cell r="D128">
-            <v>30</v>
-          </cell>
-          <cell r="E128">
-            <v>49</v>
-          </cell>
-          <cell r="F128">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="C129">
-            <v>38</v>
-          </cell>
-          <cell r="D129">
-            <v>31</v>
-          </cell>
-          <cell r="E129">
-            <v>53</v>
-          </cell>
-          <cell r="F129">
-            <v>14</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="C130">
-            <v>40</v>
-          </cell>
-          <cell r="D130">
-            <v>33</v>
-          </cell>
-          <cell r="E130">
-            <v>57</v>
-          </cell>
-          <cell r="F130">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="C131">
-            <v>43</v>
-          </cell>
-          <cell r="D131">
-            <v>35</v>
-          </cell>
-          <cell r="E131">
-            <v>63</v>
-          </cell>
-          <cell r="F131">
-            <v>16</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="C132">
-            <v>44</v>
-          </cell>
-          <cell r="D132">
-            <v>35</v>
-          </cell>
-          <cell r="E132">
-            <v>65</v>
-          </cell>
-          <cell r="F132">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="C133">
-            <v>46</v>
-          </cell>
-          <cell r="D133">
-            <v>36</v>
-          </cell>
-          <cell r="E133">
-            <v>70</v>
-          </cell>
-          <cell r="F133">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="C134">
-            <v>48</v>
-          </cell>
-          <cell r="D134">
-            <v>38</v>
-          </cell>
-          <cell r="E134">
-            <v>73</v>
-          </cell>
-          <cell r="F134">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="C135">
-            <v>52</v>
-          </cell>
-          <cell r="D135">
-            <v>41</v>
-          </cell>
-          <cell r="E135">
-            <v>79</v>
-          </cell>
-          <cell r="F135">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="136">
-          <cell r="C136">
-            <v>50</v>
-          </cell>
-          <cell r="D136">
-            <v>40</v>
-          </cell>
-          <cell r="E136">
-            <v>76</v>
-          </cell>
-          <cell r="F136">
-            <v>21</v>
-          </cell>
-        </row>
-        <row r="137">
-          <cell r="C137">
-            <v>50</v>
-          </cell>
-          <cell r="D137">
-            <v>40</v>
-          </cell>
-          <cell r="E137">
-            <v>76</v>
-          </cell>
-          <cell r="F137">
-            <v>22</v>
-          </cell>
-        </row>
-        <row r="138">
-          <cell r="C138">
-            <v>51</v>
-          </cell>
-          <cell r="D138">
-            <v>41</v>
-          </cell>
-          <cell r="E138">
-            <v>76</v>
-          </cell>
-          <cell r="F138">
-            <v>23</v>
-          </cell>
-        </row>
-        <row r="139">
-          <cell r="C139">
-            <v>51</v>
-          </cell>
-          <cell r="D139">
-            <v>41</v>
-          </cell>
-          <cell r="E139">
-            <v>76</v>
-          </cell>
-          <cell r="F139">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="140">
-          <cell r="C140">
-            <v>52</v>
-          </cell>
-          <cell r="D140">
-            <v>42</v>
-          </cell>
-          <cell r="E140">
-            <v>76</v>
-          </cell>
-          <cell r="F140">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="141">
-          <cell r="C141">
-            <v>53</v>
-          </cell>
-          <cell r="D141">
-            <v>42</v>
-          </cell>
-          <cell r="E141">
-            <v>77</v>
-          </cell>
-          <cell r="F141">
-            <v>26</v>
-          </cell>
-        </row>
-        <row r="142">
-          <cell r="C142">
-            <v>51</v>
-          </cell>
-          <cell r="D142">
-            <v>41</v>
-          </cell>
-          <cell r="E142">
-            <v>75</v>
-          </cell>
-          <cell r="F142">
-            <v>27</v>
-          </cell>
-        </row>
-        <row r="143">
-          <cell r="C143">
-            <v>48</v>
-          </cell>
-          <cell r="D143">
-            <v>39</v>
-          </cell>
-          <cell r="E143">
-            <v>66</v>
-          </cell>
-          <cell r="F143">
-            <v>28</v>
-          </cell>
-        </row>
-        <row r="144">
-          <cell r="C144">
-            <v>41</v>
-          </cell>
-          <cell r="D144">
-            <v>35</v>
-          </cell>
-          <cell r="E144">
-            <v>57</v>
-          </cell>
-          <cell r="F144">
-            <v>29</v>
-          </cell>
-        </row>
-        <row r="145">
-          <cell r="C145">
-            <v>36</v>
-          </cell>
-          <cell r="D145">
-            <v>31</v>
-          </cell>
-          <cell r="E145">
-            <v>47</v>
-          </cell>
-          <cell r="F145">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="C146">
-            <v>34</v>
-          </cell>
-          <cell r="D146">
-            <v>29</v>
-          </cell>
-          <cell r="E146">
-            <v>43</v>
-          </cell>
-          <cell r="F146">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="C147">
-            <v>33</v>
-          </cell>
-          <cell r="D147">
-            <v>29</v>
-          </cell>
-          <cell r="E147">
-            <v>40</v>
-          </cell>
-          <cell r="F147">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="C148">
-            <v>32</v>
-          </cell>
-          <cell r="D148">
-            <v>29</v>
-          </cell>
-          <cell r="E148">
-            <v>39</v>
-          </cell>
-          <cell r="F148">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="C149">
-            <v>31</v>
-          </cell>
-          <cell r="D149">
-            <v>28</v>
-          </cell>
-          <cell r="E149">
-            <v>38</v>
-          </cell>
-          <cell r="F149">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="C150">
-            <v>33</v>
-          </cell>
-          <cell r="D150">
-            <v>29</v>
-          </cell>
-          <cell r="E150">
-            <v>39</v>
-          </cell>
-          <cell r="F150">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="C151">
-            <v>34</v>
-          </cell>
-          <cell r="D151">
-            <v>28</v>
-          </cell>
-          <cell r="E151">
-            <v>44</v>
-          </cell>
-          <cell r="F151">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="C152">
-            <v>35</v>
-          </cell>
-          <cell r="D152">
-            <v>29</v>
-          </cell>
-          <cell r="E152">
-            <v>46</v>
-          </cell>
-          <cell r="F152">
-            <v>14</v>
-          </cell>
-        </row>
-        <row r="153">
-          <cell r="C153">
-            <v>38</v>
-          </cell>
-          <cell r="D153">
-            <v>31</v>
-          </cell>
-          <cell r="E153">
-            <v>52</v>
-          </cell>
-          <cell r="F153">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="154">
-          <cell r="C154">
-            <v>40</v>
-          </cell>
-          <cell r="D154">
-            <v>33</v>
-          </cell>
-          <cell r="E154">
-            <v>56</v>
-          </cell>
-          <cell r="F154">
-            <v>16</v>
-          </cell>
-        </row>
-        <row r="155">
-          <cell r="C155">
-            <v>45</v>
-          </cell>
-          <cell r="D155">
-            <v>36</v>
-          </cell>
-          <cell r="E155">
-            <v>65</v>
-          </cell>
-          <cell r="F155">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="156">
-          <cell r="C156">
-            <v>47</v>
-          </cell>
-          <cell r="D156">
-            <v>37</v>
-          </cell>
-          <cell r="E156">
-            <v>70</v>
-          </cell>
-          <cell r="F156">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="157">
-          <cell r="C157">
-            <v>49</v>
-          </cell>
-          <cell r="D157">
-            <v>38</v>
-          </cell>
-          <cell r="E157">
-            <v>73</v>
-          </cell>
-          <cell r="F157">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="158">
-          <cell r="C158">
-            <v>51</v>
-          </cell>
-          <cell r="D158">
-            <v>40</v>
-          </cell>
-          <cell r="E158">
-            <v>76</v>
-          </cell>
-          <cell r="F158">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="159">
-          <cell r="C159">
-            <v>51</v>
-          </cell>
-          <cell r="D159">
-            <v>41</v>
-          </cell>
-          <cell r="E159">
-            <v>78</v>
-          </cell>
-          <cell r="F159">
-            <v>21</v>
-          </cell>
-        </row>
-        <row r="160">
-          <cell r="C160">
-            <v>51</v>
-          </cell>
-          <cell r="D160">
-            <v>41</v>
-          </cell>
-          <cell r="E160">
-            <v>77</v>
-          </cell>
-          <cell r="F160">
-            <v>22</v>
-          </cell>
-        </row>
-        <row r="161">
-          <cell r="C161">
-            <v>50</v>
-          </cell>
-          <cell r="D161">
-            <v>40</v>
-          </cell>
-          <cell r="E161">
-            <v>74</v>
-          </cell>
-          <cell r="F161">
-            <v>23</v>
-          </cell>
-        </row>
-        <row r="162">
-          <cell r="C162">
-            <v>50</v>
-          </cell>
-          <cell r="D162">
-            <v>41</v>
-          </cell>
-          <cell r="E162">
-            <v>73</v>
-          </cell>
-          <cell r="F162">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="163">
-          <cell r="C163">
-            <v>49</v>
-          </cell>
-          <cell r="D163">
-            <v>40</v>
-          </cell>
-          <cell r="E163">
-            <v>71</v>
-          </cell>
-          <cell r="F163">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="164">
-          <cell r="C164">
-            <v>48</v>
-          </cell>
-          <cell r="D164">
-            <v>39</v>
-          </cell>
-          <cell r="E164">
-            <v>68</v>
-          </cell>
-          <cell r="F164">
-            <v>26</v>
-          </cell>
-        </row>
-        <row r="165">
-          <cell r="C165">
-            <v>46</v>
-          </cell>
-          <cell r="D165">
-            <v>37</v>
-          </cell>
-          <cell r="E165">
-            <v>66</v>
-          </cell>
-          <cell r="F165">
-            <v>27</v>
-          </cell>
-        </row>
-        <row r="166">
-          <cell r="C166">
-            <v>43</v>
-          </cell>
-          <cell r="D166">
-            <v>36</v>
-          </cell>
-          <cell r="E166">
-            <v>60</v>
-          </cell>
-          <cell r="F166">
-            <v>28</v>
-          </cell>
-        </row>
-        <row r="167">
-          <cell r="C167">
-            <v>39</v>
-          </cell>
-          <cell r="D167">
-            <v>32</v>
-          </cell>
-          <cell r="E167">
-            <v>52</v>
-          </cell>
-          <cell r="F167">
-            <v>29</v>
-          </cell>
-        </row>
-        <row r="168">
-          <cell r="C168">
-            <v>35</v>
-          </cell>
-          <cell r="D168">
-            <v>30</v>
-          </cell>
-          <cell r="E168">
-            <v>46</v>
-          </cell>
-          <cell r="F168">
-            <v>30</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11322,8 +8953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G54" workbookViewId="0">
-      <selection activeCell="Y65" sqref="Y65"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Y43" sqref="Y43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>